<commit_message>
fix font size in new magazine
</commit_message>
<xml_diff>
--- a/dist/agree.xlsx
+++ b/dist/agree.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EEE278-896D-490D-B79E-2335F66102AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6C268A-0F9D-4E60-B615-A40E0CACCE09}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -973,35 +973,35 @@
   </sheetPr>
   <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" customWidth="1"/>
-    <col min="2" max="2" width="4.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7.109375" customWidth="1"/>
-    <col min="5" max="5" width="3.44140625" customWidth="1"/>
-    <col min="6" max="6" width="4.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" customWidth="1"/>
-    <col min="9" max="9" width="3.44140625" customWidth="1"/>
-    <col min="10" max="10" width="4.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="7.109375" customWidth="1"/>
-    <col min="13" max="13" width="3.44140625" customWidth="1"/>
-    <col min="14" max="14" width="4.33203125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="13.109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="7.109375" customWidth="1"/>
-    <col min="17" max="17" width="3.44140625" customWidth="1"/>
-    <col min="18" max="18" width="4.33203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.109375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="7.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" customWidth="1"/>
+    <col min="5" max="5" width="3.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" customWidth="1"/>
+    <col min="13" max="13" width="3.42578125" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" customWidth="1"/>
+    <col min="17" max="17" width="3.42578125" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="4" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="4" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
         <v>6</v>
       </c>
@@ -1025,7 +1025,7 @@
       <c r="S1" s="51"/>
       <c r="T1" s="51"/>
     </row>
-    <row r="2" spans="1:20" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1119,7 +1119,7 @@
       <c r="S3" s="18"/>
       <c r="T3" s="15"/>
     </row>
-    <row r="4" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="19">
         <v>2</v>
       </c>
@@ -1151,7 +1151,7 @@
       <c r="S4" s="22"/>
       <c r="T4" s="20"/>
     </row>
-    <row r="5" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="19">
         <v>3</v>
       </c>
@@ -1183,7 +1183,7 @@
       <c r="S5" s="22"/>
       <c r="T5" s="20"/>
     </row>
-    <row r="6" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24">
         <v>4</v>
       </c>
@@ -1215,7 +1215,7 @@
       <c r="S6" s="22"/>
       <c r="T6" s="20"/>
     </row>
-    <row r="7" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19">
         <v>5</v>
       </c>
@@ -1247,7 +1247,7 @@
       <c r="S7" s="22"/>
       <c r="T7" s="20"/>
     </row>
-    <row r="8" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19">
         <v>6</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="S8" s="22"/>
       <c r="T8" s="20"/>
     </row>
-    <row r="9" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24">
         <v>7</v>
       </c>
@@ -1311,7 +1311,7 @@
       <c r="S9" s="22"/>
       <c r="T9" s="20"/>
     </row>
-    <row r="10" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19">
         <v>8</v>
       </c>
@@ -1343,7 +1343,7 @@
       <c r="S10" s="25"/>
       <c r="T10" s="20"/>
     </row>
-    <row r="11" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19">
         <v>9</v>
       </c>
@@ -1375,7 +1375,7 @@
       <c r="S11" s="22"/>
       <c r="T11" s="20"/>
     </row>
-    <row r="12" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="24">
         <v>10</v>
       </c>
@@ -1407,7 +1407,7 @@
       <c r="S12" s="27"/>
       <c r="T12" s="20"/>
     </row>
-    <row r="13" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19">
         <v>11</v>
       </c>
@@ -1439,7 +1439,7 @@
       <c r="S13" s="28"/>
       <c r="T13" s="20"/>
     </row>
-    <row r="14" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="19">
         <v>12</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="S14" s="30"/>
       <c r="T14" s="20"/>
     </row>
-    <row r="15" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="24">
         <v>13</v>
       </c>
@@ -1503,7 +1503,7 @@
       <c r="S15" s="32"/>
       <c r="T15" s="20"/>
     </row>
-    <row r="16" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19">
         <v>14</v>
       </c>
@@ -1535,7 +1535,7 @@
       <c r="S16" s="32"/>
       <c r="T16" s="20"/>
     </row>
-    <row r="17" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19">
         <v>15</v>
       </c>
@@ -1567,7 +1567,7 @@
       <c r="S17" s="32"/>
       <c r="T17" s="20"/>
     </row>
-    <row r="18" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="24">
         <v>16</v>
       </c>
@@ -1599,7 +1599,7 @@
       <c r="S18" s="32"/>
       <c r="T18" s="20"/>
     </row>
-    <row r="19" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19">
         <v>17</v>
       </c>
@@ -1631,7 +1631,7 @@
       <c r="S19" s="32"/>
       <c r="T19" s="20"/>
     </row>
-    <row r="20" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19">
         <v>18</v>
       </c>
@@ -1663,7 +1663,7 @@
       <c r="S20" s="32"/>
       <c r="T20" s="20"/>
     </row>
-    <row r="21" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="24">
         <v>19</v>
       </c>
@@ -1695,7 +1695,7 @@
       <c r="S21" s="32"/>
       <c r="T21" s="20"/>
     </row>
-    <row r="22" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="19">
         <v>20</v>
       </c>
@@ -1727,7 +1727,7 @@
       <c r="S22" s="32"/>
       <c r="T22" s="20"/>
     </row>
-    <row r="23" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19">
         <v>21</v>
       </c>
@@ -1759,7 +1759,7 @@
       <c r="S23" s="32"/>
       <c r="T23" s="20"/>
     </row>
-    <row r="24" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="24">
         <v>22</v>
       </c>
@@ -1791,7 +1791,7 @@
       <c r="S24" s="32"/>
       <c r="T24" s="20"/>
     </row>
-    <row r="25" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="19">
         <v>23</v>
       </c>
@@ -1823,7 +1823,7 @@
       <c r="S25" s="32"/>
       <c r="T25" s="20"/>
     </row>
-    <row r="26" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19">
         <v>24</v>
       </c>
@@ -1855,7 +1855,7 @@
       <c r="S26" s="32"/>
       <c r="T26" s="20"/>
     </row>
-    <row r="27" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="24">
         <v>25</v>
       </c>
@@ -1887,7 +1887,7 @@
       <c r="S27" s="32"/>
       <c r="T27" s="20"/>
     </row>
-    <row r="28" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="19">
         <v>26</v>
       </c>
@@ -1919,7 +1919,7 @@
       <c r="S28" s="32"/>
       <c r="T28" s="20"/>
     </row>
-    <row r="29" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="19">
         <v>27</v>
       </c>
@@ -1951,7 +1951,7 @@
       <c r="S29" s="32"/>
       <c r="T29" s="20"/>
     </row>
-    <row r="30" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="24">
         <v>28</v>
       </c>
@@ -1983,7 +1983,7 @@
       <c r="S30" s="32"/>
       <c r="T30" s="20"/>
     </row>
-    <row r="31" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="19">
         <v>29</v>
       </c>
@@ -2015,7 +2015,7 @@
       <c r="S31" s="32"/>
       <c r="T31" s="20"/>
     </row>
-    <row r="32" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="19">
         <v>30</v>
       </c>
@@ -2047,7 +2047,7 @@
       <c r="S32" s="32"/>
       <c r="T32" s="20"/>
     </row>
-    <row r="33" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="38">
         <v>31</v>
       </c>
@@ -2079,7 +2079,7 @@
       <c r="S33" s="32"/>
       <c r="T33" s="20"/>
     </row>
-    <row r="34" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="19">
         <v>32</v>
       </c>
@@ -2111,7 +2111,7 @@
       <c r="S34" s="32"/>
       <c r="T34" s="20"/>
     </row>
-    <row r="35" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="19">
         <v>33</v>
       </c>
@@ -2143,7 +2143,7 @@
       <c r="S35" s="32"/>
       <c r="T35" s="20"/>
     </row>
-    <row r="36" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="24">
         <v>34</v>
       </c>
@@ -2175,7 +2175,7 @@
       <c r="S36" s="32"/>
       <c r="T36" s="20"/>
     </row>
-    <row r="37" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="19">
         <v>35</v>
       </c>
@@ -2207,7 +2207,7 @@
       <c r="S37" s="32"/>
       <c r="T37" s="20"/>
     </row>
-    <row r="38" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="19">
         <v>36</v>
       </c>
@@ -2239,7 +2239,7 @@
       <c r="S38" s="32"/>
       <c r="T38" s="20"/>
     </row>
-    <row r="39" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="24">
         <v>37</v>
       </c>
@@ -2271,7 +2271,7 @@
       <c r="S39" s="32"/>
       <c r="T39" s="20"/>
     </row>
-    <row r="40" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="19">
         <v>38</v>
       </c>
@@ -2303,7 +2303,7 @@
       <c r="S40" s="42"/>
       <c r="T40" s="20"/>
     </row>
-    <row r="41" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="19">
         <v>39</v>
       </c>
@@ -2335,7 +2335,7 @@
       <c r="S41" s="32"/>
       <c r="T41" s="20"/>
     </row>
-    <row r="42" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="24">
         <v>40</v>
       </c>
@@ -2367,7 +2367,7 @@
       <c r="S42" s="32"/>
       <c r="T42" s="20"/>
     </row>
-    <row r="43" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="19">
         <v>41</v>
       </c>
@@ -2399,7 +2399,7 @@
       <c r="S43" s="32"/>
       <c r="T43" s="20"/>
     </row>
-    <row r="44" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="19">
         <v>42</v>
       </c>
@@ -2431,7 +2431,7 @@
       <c r="S44" s="32"/>
       <c r="T44" s="20"/>
     </row>
-    <row r="45" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="24">
         <v>43</v>
       </c>
@@ -2463,7 +2463,7 @@
       <c r="S45" s="32"/>
       <c r="T45" s="20"/>
     </row>
-    <row r="46" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="19">
         <v>44</v>
       </c>
@@ -2495,7 +2495,7 @@
       <c r="S46" s="32"/>
       <c r="T46" s="20"/>
     </row>
-    <row r="47" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="19">
         <v>45</v>
       </c>
@@ -2527,7 +2527,7 @@
       <c r="S47" s="42"/>
       <c r="T47" s="20"/>
     </row>
-    <row r="48" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="24">
         <v>46</v>
       </c>
@@ -2559,7 +2559,7 @@
       <c r="S48" s="32"/>
       <c r="T48" s="20"/>
     </row>
-    <row r="49" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="19">
         <v>47</v>
       </c>
@@ -2591,7 +2591,7 @@
       <c r="S49" s="32"/>
       <c r="T49" s="20"/>
     </row>
-    <row r="50" spans="1:20" s="11" customFormat="1" ht="10.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" s="11" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="43">
         <v>48</v>
       </c>
@@ -2623,7 +2623,7 @@
       <c r="S50" s="50"/>
       <c r="T50" s="44"/>
     </row>
-    <row r="51" spans="1:20" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="52" t="s">
         <v>4</v>
       </c>
@@ -2647,7 +2647,7 @@
       <c r="S51" s="52"/>
       <c r="T51" s="52"/>
     </row>
-    <row r="52" spans="1:20" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="53" t="s">
         <v>5</v>
       </c>
@@ -2678,6 +2678,6 @@
     <mergeCell ref="A52:T52"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="86" orientation="landscape" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>